<commit_message>
results with fixed workflow
</commit_message>
<xml_diff>
--- a/results/escherichia_coli/Cra_Crp_Study/BAR_condition-specific_enrichment_analysis.xlsx
+++ b/results/escherichia_coli/Cra_Crp_Study/BAR_condition-specific_enrichment_analysis.xlsx
@@ -7,11 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_ac_e3.33_Presence" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_ac_e3.33-deletion_Cra_Presence" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_fru_e10.0_Presence" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_fru_e10.0-deletion_Cra_Presence" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_glc__D_e10.0-deletion_Cra_Presence" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_ac_e3.33" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_ac_e3.33-deletion_Cra" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_fru_e10.0" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_fru_e10.0-deletion_Cra" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_glc__D_e10.0-deletion_Cra" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -469,260 +469,260 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6.924932188651755e-84</v>
+        <v>1.604968443914633e-32</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7877094972067039</v>
+        <v>0.6301369863013698</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7877094972067039</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Oxidative Phosphorylation</t>
+          <t>Membrane Lipid Metabolism</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>7.863993526518334e-19</v>
+        <v>3.120649350064958e-15</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5353535353535354</v>
+        <v>0.8536585365853658</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5353535353535354</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Citric Acid Cycle</t>
+          <t>Purine and Pyrimidine Biosynthesis</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.229788606854534e-18</v>
+        <v>1.688603250476145e-10</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cell Envelope Biosynthesis</t>
+          <t>Citric Acid Cycle</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9.237337579068264e-17</v>
+        <v>8.036603046940689e-09</v>
       </c>
       <c r="D5" t="n">
-        <v>0.660377358490566</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.660377358490566</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tyrosine, Tryptophan, and Phenylalanine Metabolism</t>
+          <t>Valine, Leucine, and Isoleucine Metabolism</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.483966490250713e-16</v>
+        <v>2.542156093670281e-08</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9375</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9166666666666666</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
+          <t>Tyrosine, Tryptophan, and Phenylalanine Metabolism</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.205068715716242e-15</v>
+        <v>3.06702907152471e-07</v>
       </c>
       <c r="D7" t="n">
-        <v>0.625</v>
+        <v>0.7826086956521739</v>
       </c>
       <c r="E7" t="n">
-        <v>0.625</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Purine and Pyrimidine Biosynthesis</t>
+          <t>Arginine and Proline Metabolism</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9.07330663164552e-15</v>
+        <v>1.669562956119269e-06</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.625</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9090909090909091</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Inorganic Ion Transport and Metabolism</t>
+          <t>Histidine Metabolism</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.046805647232134e-13</v>
+        <v>1.687793982397576e-06</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5061728395061729</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5061728395061729</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Arginine and Proline Metabolism</t>
+          <t>Glycolysis/Gluconeogenesis</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3.774741307070684e-13</v>
+        <v>5.03983769554663e-05</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6585365853658537</v>
+        <v>0.6818181818181818</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6585365853658537</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Valine, Leucine, and Isoleucine Metabolism</t>
+          <t>Threonine and Lysine Metabolism</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>6.58480796890037e-13</v>
+        <v>0.0001568547794907043</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Membrane Lipid Metabolism</t>
+          <t>Murein Biosynthesis</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>6.58480796890037e-13</v>
+        <v>0.0002019906549101452</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Glycolysis/Gluconeogenesis</t>
+          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3.609115416946926e-12</v>
+        <v>0.0005165544186764511</v>
       </c>
       <c r="D13" t="n">
-        <v>0.696969696969697</v>
+        <v>0.4507042253521127</v>
       </c>
       <c r="E13" t="n">
-        <v>0.696969696969697</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Threonine and Lysine Metabolism</t>
+          <t>Pyruvate Metabolism</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.621355912117004e-10</v>
+        <v>0.0006416478334034721</v>
       </c>
       <c r="D14" t="n">
         <v>0.8</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Murein Biosynthesis</t>
+          <t>Methionine Metabolism</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>7.820288081822988e-09</v>
+        <v>0.001301664712241185</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
@@ -731,326 +731,326 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nucleotide Salvage Pathway</t>
+          <t>Alanine and Aspartate Metabolism</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.919223569836947e-08</v>
+        <v>0.001962460046423446</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4155844155844156</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4155844155844156</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Histidine Metabolism</t>
+          <t>Glyoxylate Metabolism</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.086818965916438e-08</v>
+        <v>0.004972092176911481</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Methionine Metabolism</t>
+          <t>Cysteine Metabolism</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5.305026690280583e-08</v>
+        <v>0.008319673190559677</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Pyruvate Metabolism</t>
+          <t>Anaplerotic Reactions</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.924797127671454e-07</v>
+        <v>0.03516651912445177</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5128205128205128</v>
+        <v>0.625</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5128205128205128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Alanine and Aspartate Metabolism</t>
+          <t>Glutamate Metabolism</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3.821823743829347e-07</v>
+        <v>0.04646245715385962</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8333333333333334</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Pentose Phosphate Pathway</t>
+          <t>Intracellular demand</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8.950265455091038e-07</v>
+        <v>0.04646245715385962</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E21" t="n">
-        <v>0.7333333333333333</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Transport, Outer Membrane Porin</t>
+          <t>Glycine and Serine Metabolism</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.143823823110259e-06</v>
+        <v>0.05181153925369161</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Cysteine Metabolism</t>
+          <t>Biomass and maintenance functions</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3.558531629655184e-06</v>
+        <v>0.06010125455950895</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5600000000000001</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Glycine and Serine Metabolism</t>
+          <t>Oxidative Phosphorylation</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.109586287347973e-05</v>
+        <v>0.1236158585370093</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.3461538461538461</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6666666666666666</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Glycerophospholipid Metabolism</t>
+          <t>Pentose Phosphate Pathway</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.313483173561327e-05</v>
+        <v>0.1918502478345474</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5416666666666666</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Glutamate Metabolism</t>
+          <t>Folate Metabolism</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3.509445018843793e-05</v>
+        <v>0.1964605167275343</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E26" t="n">
-        <v>0.7272727272727273</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Alternate Carbon Metabolism</t>
+          <t>Cell Envelope Biosynthesis</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4.630632986361184e-05</v>
+        <v>0.2797827220024195</v>
       </c>
       <c r="D27" t="n">
-        <v>0.2696629213483146</v>
+        <v>0.291044776119403</v>
       </c>
       <c r="E27" t="n">
-        <v>0.2696629213483146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Anaplerotic Reactions</t>
+          <t>Nucleotide Salvage Pathway</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.000166754343879384</v>
+        <v>0.7508612379452616</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7</v>
+        <v>0.2446043165467626</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Inorganic Ion Transport and Metabolism</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.003657553912768236</v>
+        <v>0.877494256588123</v>
       </c>
       <c r="D29" t="n">
-        <v>0.3529411764705883</v>
+        <v>0.2232142857142857</v>
       </c>
       <c r="E29" t="n">
-        <v>0.3529411764705883</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Folate Metabolism</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.01143820721717205</v>
+        <v>0.9832804322061256</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5</v>
+        <v>0.1153846153846154</v>
       </c>
       <c r="E30" t="n">
-        <v>0.5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Glyoxylate Metabolism</t>
+          <t>Murein Recycling</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.01325245704195416</v>
+        <v>0.9961857108081743</v>
       </c>
       <c r="D31" t="n">
-        <v>0.75</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="E31" t="n">
-        <v>0.75</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Biomass and maintenance functions</t>
+          <t>Alternate Carbon Metabolism</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.02416304769038899</v>
+        <v>0.9978033436107625</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0.1846153846153846</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1058,79 +1058,79 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.1576913894298583</v>
+        <v>0.9999896264886564</v>
       </c>
       <c r="D33" t="n">
-        <v>0.25</v>
+        <v>0.04347826086956522</v>
       </c>
       <c r="E33" t="n">
-        <v>0.25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Murein Recycling</t>
+          <t>Glycerophospholipid Metabolism</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.6819097375019159</v>
+        <v>0.9999999999205458</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1097560975609756</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1379310344827586</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Methylglyoxal Metabolism</t>
+          <t>Transport, Inner Membrane</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.7417267139741145</v>
+        <v>0.9999999999994441</v>
       </c>
       <c r="D35" t="n">
-        <v>0.125</v>
+        <v>0.1174698795180723</v>
       </c>
       <c r="E35" t="n">
-        <v>0.125</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Nitrogen Metabolism</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
         <v>1</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Transport, Inner Membrane</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>0.9529985647959275</v>
-      </c>
       <c r="D36" t="n">
-        <v>0.1209677419354839</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1209677419354839</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Nitrogen Metabolism</t>
+          <t>Methylglyoxal Metabolism</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1140,26 +1140,64 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>tRNA Charging</t>
+          <t>Transport, Outer Membrane Porin</t>
         </is>
       </c>
       <c r="C38" t="n">
         <v>1</v>
       </c>
       <c r="D38" t="n">
+        <v>0.07777777777777778</v>
+      </c>
+      <c r="E38" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Extracellular exchange</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.06790123456790123</v>
+      </c>
+      <c r="E39" t="n">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>tRNA Charging</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
         <v>0</v>
       </c>
-      <c r="E38" t="n">
-        <v>0</v>
+      <c r="E40" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1173,7 +1211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1205,7 +1243,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1213,56 +1251,56 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.247787977295455e-86</v>
+        <v>2.759269739997459e-37</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7932960893854749</v>
+        <v>0.6575342465753424</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7932960893854749</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Oxidative Phosphorylation</t>
+          <t>Membrane Lipid Metabolism</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.351008008583989e-17</v>
+        <v>2.970696889126357e-15</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.8536585365853658</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5151515151515151</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cell Envelope Biosynthesis</t>
+          <t>Purine and Pyrimidine Biosynthesis</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4.787762849043303e-17</v>
+        <v>1.636963572304981e-10</v>
       </c>
       <c r="D4" t="n">
-        <v>0.660377358490566</v>
+        <v>0.88</v>
       </c>
       <c r="E4" t="n">
-        <v>0.660377358490566</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1270,512 +1308,512 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.597511773579321e-16</v>
+        <v>1.872930044492733e-09</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9166666666666666</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
+          <t>Arginine and Proline Metabolism</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6.312357666341716e-16</v>
+        <v>9.047767469987731e-09</v>
       </c>
       <c r="D6" t="n">
-        <v>0.625</v>
+        <v>0.7</v>
       </c>
       <c r="E6" t="n">
-        <v>0.625</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Arginine and Proline Metabolism</t>
+          <t>Valine, Leucine, and Isoleucine Metabolism</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.49821641666725e-15</v>
+        <v>2.487853409662561e-08</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7073170731707317</v>
+        <v>0.9375</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7073170731707317</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Purine and Pyrimidine Biosynthesis</t>
+          <t>Histidine Metabolism</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6.081762222502441e-15</v>
+        <v>1.663226384400524e-06</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9090909090909091</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9090909090909091</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Inorganic Ion Transport and Metabolism</t>
+          <t>Citric Acid Cycle</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8.296966811068995e-15</v>
+        <v>6.979158200329782e-05</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5185185185185185</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5185185185185185</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Valine, Leucine, and Isoleucine Metabolism</t>
+          <t>Threonine and Lysine Metabolism</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4.858675737104443e-13</v>
+        <v>0.0001543234841028733</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Membrane Lipid Metabolism</t>
+          <t>Murein Biosynthesis</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4.858675737104443e-13</v>
+        <v>0.0001991268410704697</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Glycolysis/Gluconeogenesis</t>
+          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2.337360625118511e-12</v>
+        <v>0.0005021697818623123</v>
       </c>
       <c r="D12" t="n">
-        <v>0.696969696969697</v>
+        <v>0.4507042253521127</v>
       </c>
       <c r="E12" t="n">
-        <v>0.696969696969697</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Citric Acid Cycle</t>
+          <t>Glycolysis/Gluconeogenesis</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6.43218468589392e-12</v>
+        <v>0.001239005048702829</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8181818181818182</v>
+        <v>0.5909090909090909</v>
       </c>
       <c r="E13" t="n">
-        <v>0.8181818181818182</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Threonine and Lysine Metabolism</t>
+          <t>Methionine Metabolism</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.920804666653896e-10</v>
+        <v>0.001285657811843353</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Murein Biosynthesis</t>
+          <t>Alanine and Aspartate Metabolism</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6.390721464929338e-09</v>
+        <v>0.001944170162599562</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Histidine Metabolism</t>
+          <t>Glyoxylate Metabolism</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4.242308308946773e-08</v>
+        <v>0.004943142586361776</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Alanine and Aspartate Metabolism</t>
+          <t>Pyruvate Metabolism</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3.143612412142638e-07</v>
+        <v>0.004999495018525171</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8333333333333334</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Glycine and Serine Metabolism</t>
+          <t>Cysteine Metabolism</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>7.261478406186071e-07</v>
+        <v>0.008240965312570283</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7333333333333333</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="E18" t="n">
-        <v>0.7333333333333333</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Transport, Outer Membrane Porin</t>
+          <t>Glycine and Serine Metabolism</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.861921392528474e-06</v>
+        <v>0.0148155895309007</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Pentose Phosphate Pathway</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.01972626104686902</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="E20" t="n">
         <v>12</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Pyruvate Metabolism</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>4.179783268831346e-06</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.4615384615384616</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.4615384615384616</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Pentose Phosphate Pathway</t>
+          <t>Anaplerotic Reactions</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>9.21582836780253e-06</v>
+        <v>0.03495311925032977</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.625</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6666666666666666</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Methionine Metabolism</t>
+          <t>Intracellular demand</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>9.21582836780253e-06</v>
+        <v>0.04622779287957895</v>
       </c>
       <c r="D22" t="n">
         <v>0.6666666666666666</v>
       </c>
       <c r="E22" t="n">
-        <v>0.6666666666666666</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Glycerophospholipid Metabolism</t>
+          <t>Biomass and maintenance functions</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.047166417386184e-05</v>
+        <v>0.05986051585914826</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.75</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5416666666666666</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Nucleotide Salvage Pathway</t>
+          <t>Glutamate Metabolism</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.0001058802005096422</v>
+        <v>0.1946138356497333</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3246753246753247</v>
+        <v>0.5</v>
       </c>
       <c r="E24" t="n">
-        <v>0.3246753246753247</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cysteine Metabolism</t>
+          <t>Folate Metabolism</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.0001092739081360094</v>
+        <v>0.1956782759114831</v>
       </c>
       <c r="D25" t="n">
-        <v>0.48</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E25" t="n">
-        <v>0.48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Glyoxylate Metabolism</t>
+          <t>Cell Envelope Biosynthesis</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.0005359840865081973</v>
+        <v>0.2762480353725906</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0.291044776119403</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Anaplerotic Reactions</t>
+          <t>Inorganic Ion Transport and Metabolism</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.001487406269216797</v>
+        <v>0.3457043069502518</v>
       </c>
       <c r="D27" t="n">
-        <v>0.6</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E27" t="n">
-        <v>0.6</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Glutamate Metabolism</t>
+          <t>Nucleotide Salvage Pathway</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.00285321321182121</v>
+        <v>0.4487330515129279</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.2733812949640288</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5454545454545454</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Folate Metabolism</t>
+          <t>Oxidative Phosphorylation</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.01049487089383397</v>
+        <v>0.6535595622622374</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Biomass and maintenance functions</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.02321270329771986</v>
+        <v>0.7271040705086564</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Alternate Carbon Metabolism</t>
+          <t>Murein Recycling</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.0263291164718118</v>
+        <v>0.9998905742787073</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2078651685393259</v>
+        <v>0.05263157894736842</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2078651685393259</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1783,37 +1821,37 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.06103575129826087</v>
+        <v>0.9999893887256988</v>
       </c>
       <c r="D32" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.04347826086956522</v>
       </c>
       <c r="E32" t="n">
-        <v>0.2916666666666667</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Alternate Carbon Metabolism</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.06314477974273446</v>
+        <v>0.9999999837938559</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2647058823529412</v>
+        <v>0.1128205128205128</v>
       </c>
       <c r="E33" t="n">
-        <v>0.2647058823529412</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1821,51 +1859,51 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.5150383903308819</v>
+        <v>0.9999999999980776</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1532258064516129</v>
+        <v>0.1204819277108434</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1532258064516129</v>
+        <v>332</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Methylglyoxal Metabolism</t>
+          <t>Glycerophospholipid Metabolism</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.7340681671215951</v>
+        <v>0.999999999998101</v>
       </c>
       <c r="D35" t="n">
-        <v>0.125</v>
+        <v>0.0975609756097561</v>
       </c>
       <c r="E35" t="n">
-        <v>0.125</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Murein Recycling</t>
+          <t>Transport, Outer Membrane Porin</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.9492386906636107</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="D36" t="n">
-        <v>0.06896551724137931</v>
+        <v>0.08148148148148149</v>
       </c>
       <c r="E36" t="n">
-        <v>0.06896551724137931</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37">
@@ -1884,26 +1922,64 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>tRNA Charging</t>
+          <t>Extracellular exchange</t>
         </is>
       </c>
       <c r="C38" t="n">
         <v>1</v>
       </c>
       <c r="D38" t="n">
+        <v>0.06790123456790123</v>
+      </c>
+      <c r="E38" t="n">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Methylglyoxal Metabolism</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
         <v>0</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E39" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>tRNA Charging</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
         <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1917,7 +1993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1949,7 +2025,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1957,550 +2033,550 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6.633429274574238e-86</v>
+        <v>2.468377366812157e-32</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7988826815642458</v>
+        <v>0.634703196347032</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7988826815642458</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Glycolysis/Gluconeogenesis</t>
+          <t>Membrane Lipid Metabolism</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6.690801885084819e-20</v>
+        <v>5.600385754061485e-15</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8787878787878788</v>
+        <v>0.8536585365853658</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8787878787878788</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Inorganic Ion Transport and Metabolism</t>
+          <t>Purine and Pyrimidine Biosynthesis</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9.255161361811777e-17</v>
+        <v>1.126149232136213e-11</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.92</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5555555555555556</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Purine and Pyrimidine Biosynthesis</t>
+          <t>Valine, Leucine, and Isoleucine Metabolism</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.97759561852006e-16</v>
+        <v>3.285761646674175e-08</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9545454545454546</v>
+        <v>0.9375</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9545454545454546</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tyrosine, Tryptophan, and Phenylalanine Metabolism</t>
+          <t>Glycolysis/Gluconeogenesis</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3.244649563079316e-16</v>
+        <v>1.184984598917627e-07</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9166666666666666</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
+          <t>Pentose Phosphate Pathway</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.780791173602806e-15</v>
+        <v>1.439174995978742e-07</v>
       </c>
       <c r="D7" t="n">
-        <v>0.625</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.625</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Oxidative Phosphorylation</t>
+          <t>Tyrosine, Tryptophan, and Phenylalanine Metabolism</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.072181605652205e-14</v>
+        <v>4.083268858809673e-07</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4848484848484849</v>
+        <v>0.7826086956521739</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4848484848484849</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cell Envelope Biosynthesis</t>
+          <t>Histidine Metabolism</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.376554177601131e-14</v>
+        <v>2.009170048580749e-06</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6226415094339622</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6226415094339622</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Pentose Phosphate Pathway</t>
+          <t>Citric Acid Cycle</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7.915514107076301e-13</v>
+        <v>7.436493193826224e-06</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Membrane Lipid Metabolism</t>
+          <t>Threonine and Lysine Metabolism</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.915514107076301e-13</v>
+        <v>0.0001902409109307473</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Valine, Leucine, and Isoleucine Metabolism</t>
+          <t>Alanine and Aspartate Metabolism</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>6.570120638429789e-11</v>
+        <v>0.0001914119226136491</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9333333333333333</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Citric Acid Cycle</t>
+          <t>Murein Biosynthesis</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2.263441927114663e-10</v>
+        <v>0.0002392918992365077</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7727272727272727</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="E13" t="n">
-        <v>0.7727272727272727</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Threonine and Lysine Metabolism</t>
+          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3.163877208138186e-10</v>
+        <v>0.0007205101703074395</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8</v>
+        <v>0.4507042253521127</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Murein Biosynthesis</t>
+          <t>Pyruvate Metabolism</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8.837075353958949e-09</v>
+        <v>0.0007295866214811037</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Alanine and Aspartate Metabolism</t>
+          <t>Anaplerotic Reactions</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1.413790015930516e-08</v>
+        <v>0.006421553129894591</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.75</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9166666666666666</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Histidine Metabolism</t>
+          <t>Methionine Metabolism</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.677888476656805e-08</v>
+        <v>0.007262946864291701</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Pyruvate Metabolism</t>
+          <t>Cysteine Metabolism</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.365659042820736e-07</v>
+        <v>0.009311951561225188</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5128205128205128</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5128205128205128</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Methionine Metabolism</t>
+          <t>Arginine and Proline Metabolism</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.015676938417321e-06</v>
+        <v>0.01061895976928539</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7333333333333333</v>
+        <v>0.45</v>
       </c>
       <c r="E19" t="n">
-        <v>0.7333333333333333</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Nucleotide Salvage Pathway</t>
+          <t>Oxidative Phosphorylation</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2.027523474718796e-06</v>
+        <v>0.04685574830791136</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3766233766233766</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3766233766233766</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Transport, Outer Membrane Porin</t>
+          <t>Intracellular demand</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2.334875972446972e-06</v>
+        <v>0.0493395876794419</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Arginine and Proline Metabolism</t>
+          <t>Glycine and Serine Metabolism</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3.432610961809347e-06</v>
+        <v>0.05646869837286161</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4634146341463415</v>
+        <v>0.5</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4634146341463415</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Cysteine Metabolism</t>
+          <t>Biomass and maintenance functions</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4.130282860093721e-06</v>
+        <v>0.06303509092381655</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5600000000000001</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Anaplerotic Reactions</t>
+          <t>Folate Metabolism</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.217105197771456e-05</v>
+        <v>0.06644965525536765</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E24" t="n">
-        <v>0.8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Folate Metabolism</t>
+          <t>Glyoxylate Metabolism</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.217105197771456e-05</v>
+        <v>0.2968793501384284</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="E25" t="n">
-        <v>0.8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Glycine and Serine Metabolism</t>
+          <t>Cell Envelope Biosynthesis</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1.241366306562875e-05</v>
+        <v>0.3974886948676246</v>
       </c>
       <c r="D26" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.2835820895522388</v>
       </c>
       <c r="E26" t="n">
-        <v>0.6666666666666666</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Glycerophospholipid Metabolism</t>
+          <t>Inorganic Ion Transport and Metabolism</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1.506009901370533e-05</v>
+        <v>0.4773744950686757</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.2767857142857143</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5416666666666666</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Glutamate Metabolism</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.514400586273727</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E28" t="n">
         <v>6</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Alternate Carbon Metabolism</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>6.370975439274697e-05</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.2696629213483146</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.2696629213483146</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Glutamate Metabolism</t>
+          <t>Nucleotide Salvage Pathway</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.01927138509541857</v>
+        <v>0.9470262235059762</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.2158273381294964</v>
       </c>
       <c r="E29" t="n">
-        <v>0.4545454545454545</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Biomass and maintenance functions</t>
+          <t>Murein Recycling</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.02475735137754248</v>
+        <v>0.9968070716838048</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2508,37 +2584,37 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.03193472451271404</v>
+        <v>0.9971887349284654</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2941176470588235</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2941176470588235</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Transport, Inner Membrane</t>
+          <t>Alternate Carbon Metabolism</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.04756277419916275</v>
+        <v>0.9996107531436489</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1975806451612903</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="E32" t="n">
-        <v>0.1975806451612903</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2546,98 +2622,98 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.07056745581403297</v>
+        <v>0.9999921054351785</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.04347826086956522</v>
       </c>
       <c r="E33" t="n">
-        <v>0.2916666666666667</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Glyoxylate Metabolism</t>
+          <t>Transport, Inner Membrane</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.1192695070456926</v>
+        <v>0.9999999959701893</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5</v>
+        <v>0.1475903614457831</v>
       </c>
       <c r="E34" t="n">
-        <v>0.5</v>
+        <v>332</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Murein Recycling</t>
+          <t>Glycerophospholipid Metabolism</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.6917461195285426</v>
+        <v>0.9999999999994288</v>
       </c>
       <c r="D35" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.0975609756097561</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1379310344827586</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Methylglyoxal Metabolism</t>
+          <t>Transport, Outer Membrane Porin</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.7463431250953049</v>
+        <v>0.9999999999999987</v>
       </c>
       <c r="D36" t="n">
-        <v>0.125</v>
+        <v>0.08888888888888889</v>
       </c>
       <c r="E36" t="n">
-        <v>0.125</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Nitrogen Metabolism</t>
+          <t>Extracellular exchange</t>
         </is>
       </c>
       <c r="C37" t="n">
         <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>0.07098765432098765</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>324</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>tRNA Charging</t>
+          <t>Methylglyoxal Metabolism</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -2647,7 +2723,45 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Nitrogen Metabolism</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
         <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>tRNA Charging</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2661,7 +2775,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2693,7 +2807,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2701,687 +2815,687 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7.762079367268508e-92</v>
+        <v>7.591840429416465e-37</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8435754189944135</v>
+        <v>0.684931506849315</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8435754189944135</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Oxidative Phosphorylation</t>
+          <t>Membrane Lipid Metabolism</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.727423093685678e-18</v>
+        <v>5.968426494203533e-14</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.8536585365853658</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5555555555555556</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nucleotide Salvage Pathway</t>
+          <t>Purine and Pyrimidine Biosynthesis</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3.128110263945748e-18</v>
+        <v>1.088829908543263e-09</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6103896103896104</v>
+        <v>0.88</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6103896103896104</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Inorganic Ion Transport and Metabolism</t>
+          <t>Valine, Leucine, and Isoleucine Metabolism</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7.683775269869065e-18</v>
+        <v>9.310663812192592e-08</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5925925925925926</v>
+        <v>0.9375</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5925925925925926</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Purine and Pyrimidine Biosynthesis</t>
+          <t>Nucleotide Salvage Pathway</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.050553123021169e-17</v>
+        <v>2.901538880327863e-07</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0.4892086330935252</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tyrosine, Tryptophan, and Phenylalanine Metabolism</t>
+          <t>Pentose Phosphate Pathway</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2.047855065002305e-15</v>
+        <v>3.372414813312711e-07</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9166666666666666</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9166666666666666</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cell Envelope Biosynthesis</t>
+          <t>Tyrosine, Tryptophan, and Phenylalanine Metabolism</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.966548678845126e-14</v>
+        <v>1.297176991812425e-06</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6415094339622641</v>
+        <v>0.7826086956521739</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6415094339622641</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
+          <t>Arginine and Proline Metabolism</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.585545390756399e-14</v>
+        <v>9.650989986931522e-06</v>
       </c>
       <c r="D9" t="n">
         <v>0.625</v>
       </c>
       <c r="E9" t="n">
-        <v>0.625</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Glycolysis/Gluconeogenesis</t>
+          <t>Threonine and Lysine Metabolism</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.676420004229434e-13</v>
+        <v>6.84566188669192e-05</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7575757575757576</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7575757575757576</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Membrane Lipid Metabolism</t>
+          <t>Histidine Metabolism</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2.821088670561611e-12</v>
+        <v>0.0001050342258350195</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Pentose Phosphate Pathway</t>
+          <t>Murein Biosynthesis</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2.821088670561611e-12</v>
+        <v>0.0004739680398525072</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Arginine and Proline Metabolism</t>
+          <t>Glycolysis/Gluconeogenesis</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3.761232194523553e-11</v>
+        <v>0.000747328908206729</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6341463414634146</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6341463414634146</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Valine, Leucine, and Isoleucine Metabolism</t>
+          <t>Citric Acid Cycle</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.117093374738153e-10</v>
+        <v>0.001222379927573456</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9333333333333333</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Threonine and Lysine Metabolism</t>
+          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1.155550373589723e-09</v>
+        <v>0.002629684882734085</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8</v>
+        <v>0.4507042253521127</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cysteine Metabolism</t>
+          <t>Methionine Metabolism</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1.920306336177144e-09</v>
+        <v>0.002719203703015355</v>
       </c>
       <c r="D16" t="n">
-        <v>0.72</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E16" t="n">
-        <v>0.72</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Murein Biosynthesis</t>
+          <t>Alanine and Aspartate Metabolism</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.055507807600191e-08</v>
+        <v>0.003437953774880209</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Methionine Metabolism</t>
+          <t>Glyoxylate Metabolism</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.610319291382285e-07</v>
+        <v>0.007067680784825522</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Transport, Inner Membrane</t>
+          <t>Cysteine Metabolism</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.332465570087862e-07</v>
+        <v>0.01463047681962199</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2983870967741936</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2983870967741936</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Alanine and Aspartate Metabolism</t>
+          <t>Glycine and Serine Metabolism</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>9.715178677285096e-07</v>
+        <v>0.02558874855672992</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8333333333333334</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Glycine and Serine Metabolism</t>
+          <t>Pyruvate Metabolism</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2.424357097564488e-06</v>
+        <v>0.04032528819233606</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7333333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="E21" t="n">
-        <v>0.7333333333333333</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Transport, Outer Membrane Porin</t>
+          <t>Anaplerotic Reactions</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4.210459952054542e-06</v>
+        <v>0.0505207347950281</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Histidine Metabolism</t>
+          <t>Glutamate Metabolism</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>5.465397490219342e-06</v>
+        <v>0.06285773986914218</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E23" t="n">
-        <v>0.8888888888888888</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Pyruvate Metabolism</t>
+          <t>Intracellular demand</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2.241294336081557e-05</v>
+        <v>0.06285773986914218</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4615384615384616</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E24" t="n">
-        <v>0.4615384615384616</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Glycerophospholipid Metabolism</t>
+          <t>Biomass and maintenance functions</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3.837991098107282e-05</v>
+        <v>0.0764388126647997</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.75</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5416666666666666</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Folate Metabolism</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4.785352034505312e-05</v>
+        <v>0.08706080657911236</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4705882352941176</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E26" t="n">
-        <v>0.4705882352941176</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Glutamate Metabolism</t>
+          <t>Oxidative Phosphorylation</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>7.233715205439099e-05</v>
+        <v>0.1471970155149156</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.3653846153846154</v>
       </c>
       <c r="E27" t="n">
-        <v>0.7272727272727273</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Anaplerotic Reactions</t>
+          <t>Inorganic Ion Transport and Metabolism</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.000312239655530484</v>
+        <v>0.496278295253119</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7</v>
+        <v>0.2946428571428572</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Citric Acid Cycle</t>
+          <t>Methylglyoxal Metabolism</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.0003896237074419694</v>
+        <v>0.51139306672463</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Glyoxylate Metabolism</t>
+          <t>Cell Envelope Biosynthesis</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.0008534913060949501</v>
+        <v>0.8046504942048405</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>0.2611940298507462</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Transport, Outer Membrane</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.003982990744806451</v>
+        <v>0.8114127729500419</v>
       </c>
       <c r="D31" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="E31" t="n">
-        <v>0.4166666666666667</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Folate Metabolism</t>
+          <t>Transport, Outer Membrane</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.01719065287597596</v>
+        <v>0.9971706755851372</v>
       </c>
       <c r="D32" t="n">
-        <v>0.5</v>
+        <v>0.1304347826086956</v>
       </c>
       <c r="E32" t="n">
-        <v>0.5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Alternate Carbon Metabolism</t>
+          <t>Murein Recycling</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.0236840796048739</v>
+        <v>0.999728203321771</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2303370786516854</v>
+        <v>0.07894736842105263</v>
       </c>
       <c r="E33" t="n">
-        <v>0.2303370786516854</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Biomass and maintenance functions</t>
+          <t>Alternate Carbon Metabolism</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.02928197893651454</v>
+        <v>0.9999999976671567</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>0.1230769230769231</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Methylglyoxal Metabolism</t>
+          <t>Transport, Inner Membrane</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.7777078511796391</v>
+        <v>0.9999999999903311</v>
       </c>
       <c r="D35" t="n">
-        <v>0.125</v>
+        <v>0.144578313253012</v>
       </c>
       <c r="E35" t="n">
-        <v>0.125</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Murein Recycling</t>
+          <t>Glycerophospholipid Metabolism</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.8959244053995407</v>
+        <v>0.9999999999999958</v>
       </c>
       <c r="D36" t="n">
-        <v>0.103448275862069</v>
+        <v>0.0975609756097561</v>
       </c>
       <c r="E36" t="n">
-        <v>0.103448275862069</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>tRNA Charging</t>
+          <t>Transport, Outer Membrane Porin</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.9891192294517447</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="D37" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1</v>
       </c>
       <c r="E37" t="n">
-        <v>0.04166666666666666</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Nitrogen Metabolism</t>
+          <t>tRNA Charging</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -3391,7 +3505,45 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Extracellular exchange</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.07098765432098765</v>
+      </c>
+      <c r="E39" t="n">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Nitrogen Metabolism</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
         <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3405,7 +3557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3437,7 +3589,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -3445,588 +3597,588 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7.035056656472272e-79</v>
+        <v>5.151838926107742e-31</v>
       </c>
       <c r="D2" t="n">
-        <v>0.770949720670391</v>
+        <v>0.6438356164383562</v>
       </c>
       <c r="E2" t="n">
-        <v>0.770949720670391</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Inorganic Ion Transport and Metabolism</t>
+          <t>Purine and Pyrimidine Biosynthesis</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2.160129290717558e-19</v>
+        <v>3.619376083927283e-11</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5925925925925926</v>
+        <v>0.92</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5925925925925926</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Glycolysis/Gluconeogenesis</t>
+          <t>Valine, Leucine, and Isoleucine Metabolism</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.27440490152455e-18</v>
+        <v>7.048232744599737e-08</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8484848484848485</v>
+        <v>0.9375</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8484848484848485</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Purine and Pyrimidine Biosynthesis</t>
+          <t>Cell Envelope Biosynthesis</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.041637780807863e-16</v>
+        <v>1.445009791675373e-07</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9545454545454546</v>
+        <v>0.4925373134328358</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9545454545454546</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tyrosine, Tryptophan, and Phenylalanine Metabolism</t>
+          <t>Pentose Phosphate Pathway</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3.354042289111958e-16</v>
+        <v>2.685375599840417e-07</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9166666666666666</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9166666666666666</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
+          <t>Citric Acid Cycle</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.869153426664685e-15</v>
+        <v>7.821313971189466e-07</v>
       </c>
       <c r="D7" t="n">
-        <v>0.625</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E7" t="n">
-        <v>0.625</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nucleotide Salvage Pathway</t>
+          <t>Arginine and Proline Metabolism</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2.634909257312077e-15</v>
+        <v>6.654799944381381e-06</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.625</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5454545454545454</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Citric Acid Cycle</t>
+          <t>Tyrosine, Tryptophan, and Phenylalanine Metabolism</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.191146882169659e-14</v>
+        <v>7.548588378882817e-06</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.7391304347826086</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9090909090909091</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cell Envelope Biosynthesis</t>
+          <t>Glycolysis/Gluconeogenesis</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.440689773812174e-14</v>
+        <v>2.001306222572541e-05</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6226415094339622</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6226415094339622</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Oxidative Phosphorylation</t>
+          <t>Nucleotide Salvage Pathway</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>6.016964599810438e-14</v>
+        <v>4.91299709536788e-05</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4747474747474748</v>
+        <v>0.4388489208633093</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4747474747474748</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Pentose Phosphate Pathway</t>
+          <t>Histidine Metabolism</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8.098461274420134e-13</v>
+        <v>8.915385272873565e-05</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Arginine and Proline Metabolism</t>
+          <t>Threonine and Lysine Metabolism</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5.355620563540318e-12</v>
+        <v>0.0003363452680416943</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6341463414634146</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6341463414634146</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Murein Biosynthesis</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0003951229807559334</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.7333333333333333</v>
+      </c>
+      <c r="E14" t="n">
         <v>15</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Valine, Leucine, and Isoleucine Metabolism</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>6.709886645136865e-11</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.9333333333333333</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.9333333333333333</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Threonine and Lysine Metabolism</t>
+          <t>Lipopolysaccharide Biosynthesis / Recycling</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3.238601319079014e-10</v>
+        <v>0.001877583712209938</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8</v>
+        <v>0.4507042253521127</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cysteine Metabolism</t>
+          <t>Methionine Metabolism</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4.759613456049791e-10</v>
+        <v>0.002324724594714651</v>
       </c>
       <c r="D16" t="n">
-        <v>0.72</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E16" t="n">
-        <v>0.72</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Murein Biosynthesis</t>
+          <t>Cysteine Metabolism</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>8.97219883031918e-09</v>
+        <v>0.002661807682710192</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Methionine Metabolism</t>
+          <t>Alanine and Aspartate Metabolism</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>6.214550700025373e-08</v>
+        <v>0.003049670741110364</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Glutamate Metabolism</t>
+          <t>Glyoxylate Metabolism</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>8.472651744765347e-08</v>
+        <v>0.00655355326189273</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9090909090909091</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9090909090909091</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Alanine and Aspartate Metabolism</t>
+          <t>Pyruvate Metabolism</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4.364971069700032e-07</v>
+        <v>0.007673716166773099</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8333333333333334</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Pyruvate Metabolism</t>
+          <t>Glutamate Metabolism</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.354962374451898e-06</v>
+        <v>0.008523419489179149</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4871794871794872</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="E21" t="n">
-        <v>0.4871794871794872</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Transport, Outer Membrane Porin</t>
+          <t>Glycine and Serine Metabolism</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.359752885395417e-06</v>
+        <v>0.02283672050494353</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Histidine Metabolism</t>
+          <t>Intracellular demand</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2.858561549157172e-06</v>
+        <v>0.05893524558304322</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E23" t="n">
-        <v>0.8888888888888888</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Glycine and Serine Metabolism</t>
+          <t>Biomass and maintenance functions</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.258769859431834e-05</v>
+        <v>0.07260764807616762</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.75</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6666666666666666</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Glycerophospholipid Metabolism</t>
+          <t>Folate Metabolism</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>9.261171869179691e-05</v>
+        <v>0.08104813102448762</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Membrane Lipid Metabolism</t>
+          <t>Oxidative Phosphorylation</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.0001167383529196894</v>
+        <v>0.1275296262471508</v>
       </c>
       <c r="D26" t="n">
-        <v>0.6</v>
+        <v>0.3653846153846154</v>
       </c>
       <c r="E26" t="n">
-        <v>0.6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Anaplerotic Reactions</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.0003271708955742262</v>
+        <v>0.167342870545357</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4117647058823529</v>
+        <v>0.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.4117647058823529</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Folate Metabolism</t>
+          <t>Inorganic Ion Transport and Metabolism</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.001785212496679953</v>
+        <v>0.2866787252991321</v>
       </c>
       <c r="D28" t="n">
-        <v>0.6</v>
+        <v>0.3125</v>
       </c>
       <c r="E28" t="n">
-        <v>0.6</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Transport, Outer Membrane</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.002118740274943671</v>
+        <v>0.9635479915470123</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="E29" t="n">
-        <v>0.4166666666666667</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Transport, Inner Membrane</t>
+          <t>Transport, Outer Membrane</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.02294022565609378</v>
+        <v>0.9964394179444354</v>
       </c>
       <c r="D30" t="n">
-        <v>0.2056451612903226</v>
+        <v>0.1304347826086956</v>
       </c>
       <c r="E30" t="n">
-        <v>0.2056451612903226</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Biomass and maintenance functions</t>
+          <t>Membrane Lipid Metabolism</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.02483214700103958</v>
+        <v>0.9965981954762922</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>0.1219512195121951</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Anaplerotic Reactions</t>
+          <t>Murein Recycling</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.05837295428175857</v>
+        <v>0.9996536815303447</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4</v>
+        <v>0.07894736842105263</v>
       </c>
       <c r="E32" t="n">
-        <v>0.4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -4034,13 +4186,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.09072969442582175</v>
+        <v>0.9999999999620922</v>
       </c>
       <c r="D33" t="n">
-        <v>0.1966292134831461</v>
+        <v>0.1025641025641026</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1966292134831461</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34">
@@ -4049,64 +4201,64 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Glyoxylate Metabolism</t>
+          <t>Transport, Outer Membrane Porin</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.1195882001745615</v>
+        <v>0.9999999999985226</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5</v>
+        <v>0.1185185185185185</v>
       </c>
       <c r="E34" t="n">
-        <v>0.5</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Methylglyoxal Metabolism</t>
+          <t>Glycerophospholipid Metabolism</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.7469150684434552</v>
+        <v>0.9999999999999832</v>
       </c>
       <c r="D35" t="n">
-        <v>0.125</v>
+        <v>0.0975609756097561</v>
       </c>
       <c r="E35" t="n">
-        <v>0.125</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Murein Recycling</t>
+          <t>Transport, Inner Membrane</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.8583883819408374</v>
+        <v>0.9999999999999938</v>
       </c>
       <c r="D36" t="n">
-        <v>0.103448275862069</v>
+        <v>0.1204819277108434</v>
       </c>
       <c r="E36" t="n">
-        <v>0.103448275862069</v>
+        <v>332</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Nitrogen Metabolism</t>
+          <t>tRNA Charging</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -4116,26 +4268,64 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>tRNA Charging</t>
+          <t>Extracellular exchange</t>
         </is>
       </c>
       <c r="C38" t="n">
         <v>1</v>
       </c>
       <c r="D38" t="n">
+        <v>0.08641975308641975</v>
+      </c>
+      <c r="E38" t="n">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Methylglyoxal Metabolism</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
         <v>0</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E39" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Nitrogen Metabolism</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
         <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>